<commit_message>
Excel Updates and picture
</commit_message>
<xml_diff>
--- a/Documentation/UseCases/FunctionPoints.xlsx
+++ b/Documentation/UseCases/FunctionPoints.xlsx
@@ -293,6 +293,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Finished UCs</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -355,65 +358,16 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="10"/>
-            <c:backward val="38"/>
+            <c:forward val="280"/>
+            <c:backward val="20"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.11230686789151356"/>
-                  <c:y val="0.16421296296296295"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -473,6 +427,88 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CDBF-4970-91EF-B0D1EB48AB7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>New UCs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'UCs Time and FPs'!$G$13:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>273</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'UCs Time and FPs'!$H$13:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16.9758</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.9298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.473399999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7AF2-457C-9A69-99A4B9636176}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -613,6 +649,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.73913224485797668"/>
+          <c:y val="0.63201845364043152"/>
+          <c:w val="0.17298006322724752"/>
+          <c:h val="0.13877564235391629"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1198,14 +1275,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1532,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>